<commit_message>
Fixed a malformed date.
</commit_message>
<xml_diff>
--- a/src/main/resources/Duplicates.xlsx
+++ b/src/main/resources/Duplicates.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="92">
   <si>
     <t>First Name</t>
   </si>
@@ -349,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -362,7 +362,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,7 +664,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:F29"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1105,8 +1104,8 @@
         <v>87</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="12">
-        <v>39295</v>
+      <c r="D22" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>74</v>
@@ -1223,8 +1222,8 @@
         <v>87</v>
       </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="12">
-        <v>39295</v>
+      <c r="D28" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>74</v>
@@ -1255,6 +1254,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added unkown town name.
</commit_message>
<xml_diff>
--- a/src/main/resources/Duplicates.xlsx
+++ b/src/main/resources/Duplicates.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="94">
   <si>
     <t>First Name</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>7/2/2010</t>
+  </si>
+  <si>
+    <t>Key West</t>
   </si>
   <si>
     <t>Timothy</t>
@@ -522,7 +525,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -653,24 +656,24 @@
         <v>16</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>11</v>
@@ -678,19 +681,19 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>11</v>
@@ -698,16 +701,16 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>16</v>
@@ -718,19 +721,19 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>11</v>
@@ -738,19 +741,19 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>11</v>
@@ -758,19 +761,19 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>11</v>
@@ -778,19 +781,19 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>11</v>
@@ -798,19 +801,19 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>11</v>
@@ -818,19 +821,19 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>11</v>
@@ -838,16 +841,16 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>16</v>
@@ -858,16 +861,16 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>10</v>
@@ -878,19 +881,19 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>11</v>
@@ -918,19 +921,19 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>11</v>
@@ -938,19 +941,19 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>11</v>
@@ -958,17 +961,17 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F22" s="3" t="s">
         <v>11</v>
@@ -996,19 +999,19 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>11</v>
@@ -1076,17 +1079,17 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>11</v>
@@ -1141,7 +1144,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1151,19 +1154,19 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>11</v>
@@ -1171,16 +1174,16 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>16</v>
@@ -1191,16 +1194,16 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>10</v>
@@ -1219,7 +1222,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1229,19 +1232,19 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>11</v>
@@ -1249,17 +1252,17 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="9" t="n">
         <v>39295</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>11</v>
@@ -1267,7 +1270,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1325,7 +1328,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="11" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1335,19 +1338,19 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>11</v>
@@ -1355,19 +1358,19 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Added grade names both valid and invalid.
</commit_message>
<xml_diff>
--- a/src/main/resources/Duplicates.xlsx
+++ b/src/main/resources/Duplicates.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="DataSource" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Errors" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="DataSource" sheetId="1" r:id="rId1"/>
+    <sheet name="Errors" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="97">
   <si>
     <t>First Name</t>
   </si>
@@ -298,18 +297,22 @@
   </si>
   <si>
     <t>Close Match (flag)</t>
+  </si>
+  <si>
+    <t>Grade 2</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Grade 20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -318,22 +321,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -356,104 +344,46 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -512,34 +442,322 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.4234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.9948979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.72959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.72959183673469"/>
+    <col min="1" max="1" width="11.42578125"/>
+    <col min="2" max="2" width="16.42578125"/>
+    <col min="3" max="3" width="13.140625"/>
+    <col min="4" max="4" width="12"/>
+    <col min="5" max="5" width="8.7109375"/>
+    <col min="6" max="6" width="10.85546875"/>
+    <col min="7" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -579,7 +797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -599,7 +817,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -619,7 +837,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -639,7 +857,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
@@ -659,7 +877,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>31</v>
       </c>
@@ -679,7 +897,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -699,7 +917,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -719,7 +937,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -739,7 +957,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -752,14 +970,14 @@
       <c r="D11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>48</v>
+      <c r="E11" s="12" t="s">
+        <v>95</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>49</v>
       </c>
@@ -779,7 +997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>53</v>
       </c>
@@ -799,7 +1017,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>57</v>
       </c>
@@ -819,7 +1037,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>61</v>
       </c>
@@ -839,7 +1057,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>64</v>
       </c>
@@ -859,7 +1077,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>67</v>
       </c>
@@ -879,7 +1097,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
         <v>70</v>
       </c>
@@ -899,7 +1117,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -912,14 +1130,14 @@
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>10</v>
+      <c r="E19" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>49</v>
       </c>
@@ -939,7 +1157,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
         <v>74</v>
       </c>
@@ -959,7 +1177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>78</v>
       </c>
@@ -977,7 +1195,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:6">
       <c r="A23" s="2" t="s">
         <v>17</v>
       </c>
@@ -997,7 +1215,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:6">
       <c r="A24" s="2" t="s">
         <v>36</v>
       </c>
@@ -1017,7 +1235,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:6">
       <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
@@ -1037,7 +1255,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:6">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
@@ -1050,14 +1268,14 @@
       <c r="D26" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>16</v>
+      <c r="E26" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:6">
       <c r="A27" s="2" t="s">
         <v>17</v>
       </c>
@@ -1077,7 +1295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:6">
       <c r="A28" s="2" t="s">
         <v>78</v>
       </c>
@@ -1095,7 +1313,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:6">
       <c r="A29" s="2" t="s">
         <v>17</v>
       </c>
@@ -1116,33 +1334,25 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K20" activeCellId="0" sqref="K20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.72959183673469"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
@@ -1152,7 +1362,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>81</v>
       </c>
@@ -1172,7 +1382,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6">
       <c r="A3" s="5" t="s">
         <v>85</v>
       </c>
@@ -1192,7 +1402,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6">
       <c r="A4" s="5" t="s">
         <v>88</v>
       </c>
@@ -1212,7 +1422,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -1220,7 +1430,7 @@
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6">
       <c r="A6" s="8" t="s">
         <v>91</v>
       </c>
@@ -1230,7 +1440,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="s">
         <v>74</v>
       </c>
@@ -1250,7 +1460,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
@@ -1258,7 +1468,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="D8" s="9" t="n">
+      <c r="D8" s="9">
         <v>39295</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -1268,7 +1478,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6">
       <c r="A10" s="10" t="s">
         <v>92</v>
       </c>
@@ -1278,7 +1488,7 @@
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1298,7 +1508,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
@@ -1318,7 +1528,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1326,7 +1536,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6">
       <c r="A14" s="11" t="s">
         <v>93</v>
       </c>
@@ -1336,7 +1546,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>49</v>
       </c>
@@ -1356,7 +1566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>49</v>
       </c>
@@ -1377,12 +1587,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>